<commit_message>
- combined all TC together.
</commit_message>
<xml_diff>
--- a/src/test/java/com/sovereigncs/testdata/DataProviderExp.xlsx
+++ b/src/test/java/com/sovereigncs/testdata/DataProviderExp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>FirstName</t>
   </si>
@@ -97,6 +97,30 @@
   </si>
   <si>
     <t>sovereigncs032420_1206</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_1948@test.com</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_1948</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_2008@test.com</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_2009</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_2013@test.com</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_2014</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_2015@test.com</t>
+  </si>
+  <si>
+    <t>sovereigncs032720_2015</t>
   </si>
 </sst>
 </file>
@@ -431,10 +455,10 @@
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>